<commit_message>
- Editor: Added ToolTips - lexer clean-up
</commit_message>
<xml_diff>
--- a/ProofCheckerTasks.xlsx
+++ b/ProofCheckerTasks.xlsx
@@ -38,9 +38,6 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>Make the editor invokes parser and read the tokens from the file</t>
+  </si>
+  <si>
+    <t>Done in %</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,10 +404,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -429,7 +429,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -444,7 +444,7 @@
         <v>1.2000000000000002</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -459,7 +459,7 @@
         <v>1.3000000000000003</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
- PreCommit hook - Warnings free build - Generating Tokens.cs works without any issues
</commit_message>
<xml_diff>
--- a/ProofCheckerTasks.xlsx
+++ b/ProofCheckerTasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Tasks</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Done in %</t>
+  </si>
+  <si>
+    <t>Tests are not working on x64</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>There are Win32 and x86 architectures. Need only one, probably x86</t>
   </si>
 </sst>
 </file>
@@ -386,12 +395,12 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="2" max="2" width="66.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
@@ -435,7 +444,7 @@
         <v>3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -472,12 +481,30 @@
       <c r="A6">
         <v>2</v>
       </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:A21" si="0">A6+1</f>
         <v>3</v>
       </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">

</xml_diff>